<commit_message>
*: added xlsx export.
</commit_message>
<xml_diff>
--- a/htdocs/assets/confirmations.xlsx
+++ b/htdocs/assets/confirmations.xlsx
@@ -281,7 +281,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -320,6 +320,10 @@
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -434,7 +438,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -450,7 +454,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="11.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="16.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="12.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="4" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="25.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="52.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="22.85"/>
@@ -480,7 +484,7 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
+      <c r="N1" s="10"/>
       <c r="O1" s="9"/>
       <c r="P1" s="9"/>
       <c r="Q1" s="9"/>
@@ -501,192 +505,192 @@
       <c r="AG1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="58.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="P2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="Q2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="R2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="S2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="T2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="U2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="12" t="s">
+      <c r="V2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="12" t="s">
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="AC2" s="12" t="s">
+      <c r="AC2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="AD2" s="12" t="s">
+      <c r="AD2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="AE2" s="13" t="s">
+      <c r="AE2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="AF2" s="13" t="s">
+      <c r="AF2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="AG2" s="13"/>
+      <c r="AG2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="n">
+      <c r="A3" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="n">
+      <c r="B3" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="14" t="n">
+      <c r="C3" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D3" s="15" t="n">
+      <c r="D3" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="E3" s="15" t="n">
+      <c r="E3" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="F3" s="15" t="n">
+      <c r="F3" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="G3" s="15" t="n">
+      <c r="G3" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="H3" s="15" t="n">
+      <c r="H3" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="I3" s="15" t="n">
+      <c r="I3" s="16" t="n">
         <v>9</v>
       </c>
-      <c r="J3" s="15" t="n">
+      <c r="J3" s="16" t="n">
         <v>10</v>
       </c>
-      <c r="K3" s="15" t="n">
+      <c r="K3" s="16" t="n">
         <v>11</v>
       </c>
-      <c r="L3" s="15" t="n">
+      <c r="L3" s="16" t="n">
         <v>12</v>
       </c>
-      <c r="M3" s="15" t="n">
+      <c r="M3" s="16" t="n">
         <v>13</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="O3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="15" t="s">
+      <c r="P3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="Q3" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="14" t="n">
+      <c r="R3" s="15" t="n">
         <v>18</v>
       </c>
-      <c r="S3" s="14" t="n">
+      <c r="S3" s="15" t="n">
         <v>19</v>
       </c>
-      <c r="T3" s="15" t="s">
+      <c r="T3" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="U3" s="15" t="s">
+      <c r="U3" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="V3" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="W3" s="15" t="s">
+      <c r="W3" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="X3" s="15" t="s">
+      <c r="X3" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="Y3" s="15" t="s">
+      <c r="Y3" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="Z3" s="15" t="s">
+      <c r="Z3" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="AA3" s="15" t="s">
+      <c r="AA3" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="AB3" s="15" t="s">
+      <c r="AB3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="AC3" s="15" t="s">
+      <c r="AC3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="AD3" s="15" t="s">
+      <c r="AD3" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="AE3" s="13" t="s">
+      <c r="AE3" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="AF3" s="16" t="s">
+      <c r="AF3" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="AG3" s="16" t="s">
+      <c r="AG3" s="17" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
confirmations, targets_compliance: added [succeeded] attribute.
</commit_message>
<xml_diff>
--- a/htdocs/assets/confirmations.xlsx
+++ b/htdocs/assets/confirmations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -85,6 +85,9 @@
     <t xml:space="preserve">Подтверждение выполнения</t>
   </si>
   <si>
+    <t xml:space="preserve">Задача выполнена</t>
+  </si>
+  <si>
     <t xml:space="preserve">Фото подтверждения</t>
   </si>
   <si>
@@ -155,6 +158,9 @@
   </si>
   <si>
     <t xml:space="preserve">33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34</t>
   </si>
 </sst>
 </file>
@@ -408,7 +414,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG1048576"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -438,14 +444,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="2" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="4" width="7.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="3" width="27.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="22" style="4" width="5.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="3" width="39.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="3" width="19.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="11.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="3" width="19.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="3" width="39.46"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="75" min="34" style="5" width="8.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="76" style="6" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="4" width="10.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="23" style="4" width="5.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="3" width="39.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="3" width="19.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="11.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="3" width="19.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="3" width="39.46"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="76" min="35" style="5" width="8.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="77" style="6" width="8.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="58.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -515,27 +522,30 @@
       <c r="V1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="9"/>
+      <c r="W1" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="X1" s="9"/>
       <c r="Y1" s="9"/>
       <c r="Z1" s="9"/>
       <c r="AA1" s="9"/>
-      <c r="AB1" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="AB1" s="9"/>
       <c r="AC1" s="9" t="s">
         <v>23</v>
       </c>
       <c r="AD1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" s="10" t="s">
+      <c r="AE1" s="9" t="s">
         <v>25</v>
       </c>
       <c r="AF1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AG1" s="10"/>
+      <c r="AG1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH1" s="10"/>
     </row>
     <row r="2" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="n">
@@ -578,16 +588,16 @@
         <v>13</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R2" s="11" t="n">
         <v>18</v>
@@ -596,53 +606,55 @@
         <v>19</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="V2" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="X2" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Y2" s="12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Z2" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB2" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC2" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AD2" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="AF2" s="13" t="s">
+      <c r="AE2" s="12" t="s">
         <v>43</v>
       </c>
+      <c r="AF2" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="AG2" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="AH2" s="13" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="V1:AA1"/>
-    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="W1:AB1"/>
+    <mergeCell ref="AG1:AH1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>